<commit_message>
Adicionando os loops e array de ambientes
</commit_message>
<xml_diff>
--- a/CadastroAmbientes/Meus Ambientes.xlsx
+++ b/CadastroAmbientes/Meus Ambientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e32da25853bd735/Área de Trabalho/Nova pasta/CadastroAmbientes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{AA9CF243-34F8-4EAE-99E2-89BDAE84FCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A700AB3-F860-45A3-B0F2-BBCA2E2FF59B}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{AA9CF243-34F8-4EAE-99E2-89BDAE84FCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1DE941C-D88C-4EAE-B99F-3DF1B4E6103F}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{B6A95BA2-39BD-441B-BA02-96BB9BFB940E}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{B6A95BA2-39BD-441B-BA02-96BB9BFB940E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>Unidades</t>
   </si>
   <si>
-    <t>Grupo Natureza 8033-Natureza-Carrefour Sudoeste</t>
+    <t>Teste01</t>
   </si>
 </sst>
 </file>
@@ -120,7 +120,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>